<commit_message>
Otimizados parâmetros de configuração
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -46,9 +46,6 @@
     <t>EmailPasta</t>
   </si>
   <si>
-    <t>CaminhoOutput</t>
-  </si>
-  <si>
     <t>Pasta para analisar os e-mails recebidos</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>Regex de Anexo do E-mail para separá-lo dos demais</t>
   </si>
   <si>
-    <t>AwsLogin</t>
-  </si>
-  <si>
     <t>Credenciais de acesso ao AWS</t>
   </si>
   <si>
@@ -97,13 +91,25 @@
     <t>\\Outputs\</t>
   </si>
   <si>
-    <t>BucketName</t>
-  </si>
-  <si>
     <t>Nome do bucket a serem salvos os dados</t>
   </si>
   <si>
     <t>AWS_Credencial</t>
+  </si>
+  <si>
+    <t>AWSLogin</t>
+  </si>
+  <si>
+    <t>AWSBucketName</t>
+  </si>
+  <si>
+    <t>CaminhoOutputs</t>
+  </si>
+  <si>
+    <t>EmailRemetentes</t>
+  </si>
+  <si>
+    <t>Lista de Remetentes que enviam o e-mail desejado, separados por ;</t>
   </si>
 </sst>
 </file>
@@ -477,17 +483,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z985"/>
+  <dimension ref="A1:Z986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.28515625" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -527,10 +533,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -538,13 +544,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -553,7 +559,7 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -562,76 +568,84 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
+      <c r="A6" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
+      <c r="C6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7"/>
+        <v>9</v>
+      </c>
+      <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12"/>
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="B13"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1602,6 +1616,7 @@
     <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>